<commit_message>
cycle_script: add filename, add default choise message infer_data: rename by check_sequence cycle_graphic: add ITECH ramp, time in HH:MM:SS minor fix in other_SCPI
BREAKING CHANGE: `extends` key in config file is now used for extending other config files
</commit_message>
<xml_diff>
--- a/command.xlsx
+++ b/command.xlsx
@@ -923,7 +923,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -944,189 +944,189 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B2" t="str">
         <v>ARMxl</v>
       </c>
       <c r="C2" t="str">
-        <v>set_voltage_and_power.sh</v>
+        <v>stop_charge_session.sh</v>
       </c>
       <c r="D2" t="str">
-        <v>32801</v>
+        <v>-</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B3" t="str">
-        <v>ARMxl</v>
+        <v>AC_Source</v>
       </c>
       <c r="C3" t="str">
-        <v>start_charge_session.sh</v>
+        <v>set_output</v>
       </c>
       <c r="D3" t="str">
-        <v>32916</v>
+        <v>OFF</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B4" t="str">
-        <v>ARMxl</v>
+        <v>DC_Source</v>
       </c>
       <c r="C4" t="str">
-        <v>set_power.sh</v>
+        <v>set_output</v>
       </c>
       <c r="D4" t="str">
-        <v>33095</v>
+        <v>OFF</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B5" t="str">
-        <v>ARMxl</v>
+        <v>AC_Source</v>
       </c>
       <c r="C5" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_voltage</v>
       </c>
       <c r="D5" t="str">
-        <v>33225</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>ARMxl</v>
+        <v>CLIM_chamber</v>
       </c>
       <c r="C6" t="str">
-        <v>set_reactive.sh</v>
+        <v>write_setpoint</v>
       </c>
       <c r="D6" t="str">
-        <v>33321</v>
+        <v>Temp 20</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B7" t="str">
-        <v>ARMxl</v>
+        <v>CLIM_chamber</v>
       </c>
       <c r="C7" t="str">
-        <v>set_reactive.sh</v>
+        <v>start_temp</v>
       </c>
       <c r="D7" t="str">
-        <v>33462</v>
+        <v>-</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
-        <v>ARMxl</v>
+        <v>DC_Source</v>
       </c>
       <c r="C8" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_voltage</v>
       </c>
       <c r="D8" t="str">
-        <v>33677</v>
+        <v>300</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B9" t="str">
-        <v>ARMxl</v>
+        <v>DC_Source</v>
       </c>
       <c r="C9" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_c_limit</v>
       </c>
       <c r="D9" t="str">
-        <v>33</v>
+        <v>-160 6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B10" t="str">
-        <v>ARMxl</v>
+        <v>DC_Source</v>
       </c>
       <c r="C10" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_output</v>
       </c>
       <c r="D10" t="str">
-        <v>148</v>
+        <v>ON</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B11" t="str">
-        <v>ARMxl</v>
+        <v>DC_Source</v>
       </c>
       <c r="C11" t="str">
-        <v>set_reactive.sh</v>
+        <v xml:space="preserve">set_voltage </v>
       </c>
       <c r="D11" t="str">
-        <v>327</v>
+        <v>750</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B12" t="str">
-        <v>ARMxl</v>
+        <v>AC_Source</v>
       </c>
       <c r="C12" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_output</v>
       </c>
       <c r="D12" t="str">
-        <v>457</v>
+        <v>ON</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B13" t="str">
         <v>ARMxl</v>
       </c>
       <c r="C13" t="str">
-        <v>set_reactive.sh</v>
+        <v>set_voltage_and_power.sh</v>
       </c>
       <c r="D13" t="str">
-        <v>553</v>
+        <v>8200 50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B14" t="str">
         <v>ARMxl</v>
       </c>
       <c r="C14" t="str">
-        <v>set_reactive.sh</v>
+        <v>start_charge_session.sh</v>
       </c>
       <c r="D14" t="str">
-        <v>0</v>
+        <v>-</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B15" t="str">
         <v>ARMxl</v>
@@ -1135,23 +1135,488 @@
         <v>set_power.sh</v>
       </c>
       <c r="D15" t="str">
-        <v>100</v>
+        <v>940</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>30</v>
+        <v>5400</v>
       </c>
       <c r="B16" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C16" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D16" t="str">
+        <v>Temp 25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B17" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C17" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D17" t="str">
+        <v>Temp 35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B18" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C18" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D18" t="str">
+        <v>Temp 50</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B19" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C19" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Temp 55</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B20" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C20" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D20" t="str">
+        <v>Temp 60</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B21" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C21" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D21" t="str">
+        <v>Temp 65</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B22" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C22" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D22" t="str">
+        <v>Temp 70</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B23" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C23" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D23" t="str">
+        <v>Temp 75</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>5</v>
+      </c>
+      <c r="B24" t="str">
         <v>ARMxl</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C24" t="str">
         <v>stop_charge_session.sh</v>
+      </c>
+      <c r="D24" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>5</v>
+      </c>
+      <c r="B25" t="str">
+        <v>AC_Source</v>
+      </c>
+      <c r="C25" t="str">
+        <v>set_output</v>
+      </c>
+      <c r="D25" t="str">
+        <v>OFF</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>5</v>
+      </c>
+      <c r="B26" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C26" t="str">
+        <v xml:space="preserve">set_output </v>
+      </c>
+      <c r="D26" t="str">
+        <v>OFF</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>5</v>
+      </c>
+      <c r="B27" t="str">
+        <v>AC_Source</v>
+      </c>
+      <c r="C27" t="str">
+        <v>usa_grid</v>
+      </c>
+      <c r="D27" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>5</v>
+      </c>
+      <c r="B28" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C28" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D28" t="str">
+        <v>Temp 20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>5</v>
+      </c>
+      <c r="B29" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C29" t="str">
+        <v>start_temp</v>
+      </c>
+      <c r="D29" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>5</v>
+      </c>
+      <c r="B30" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C30" t="str">
+        <v xml:space="preserve">set_voltage </v>
+      </c>
+      <c r="D30" t="str">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>5</v>
+      </c>
+      <c r="B31" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C31" t="str">
+        <v xml:space="preserve">set_c_limit </v>
+      </c>
+      <c r="D31" t="str">
+        <v>-160 6</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>10</v>
+      </c>
+      <c r="B32" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C32" t="str">
+        <v xml:space="preserve">set_output </v>
+      </c>
+      <c r="D32" t="str">
+        <v>ON</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>10</v>
+      </c>
+      <c r="B33" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C33" t="str">
+        <v xml:space="preserve">set_voltage </v>
+      </c>
+      <c r="D33" t="str">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>5</v>
+      </c>
+      <c r="B34" t="str">
+        <v>AC_Source</v>
+      </c>
+      <c r="C34" t="str">
+        <v>set_output</v>
+      </c>
+      <c r="D34" t="str">
+        <v>ON</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>5</v>
+      </c>
+      <c r="B35" t="str">
+        <v>ARMxl</v>
+      </c>
+      <c r="C35" t="str">
+        <v>set_voltage_and_power.sh</v>
+      </c>
+      <c r="D35" t="str">
+        <v>9200 50</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>5</v>
+      </c>
+      <c r="B36" t="str">
+        <v>ARMxl</v>
+      </c>
+      <c r="C36" t="str">
+        <v>start_charge_session.sh</v>
+      </c>
+      <c r="D36" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>5</v>
+      </c>
+      <c r="B37" t="str">
+        <v>ARMxl</v>
+      </c>
+      <c r="C37" t="str">
+        <v>set_power.sh</v>
+      </c>
+      <c r="D37" t="str">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>5400</v>
+      </c>
+      <c r="B38" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C38" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D38" t="str">
+        <v>Temp 25</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B39" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C39" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D39" t="str">
+        <v>Temp 35</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B40" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C40" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D40" t="str">
+        <v>Temp 50</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B41" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C41" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D41" t="str">
+        <v>Temp 55</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B42" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C42" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D42" t="str">
+        <v>Temp 60</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B43" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C43" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D43" t="str">
+        <v>Temp 65</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B44" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C44" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D44" t="str">
+        <v>Temp 70</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>2760</v>
+      </c>
+      <c r="B45" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C45" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D45" t="str">
+        <v>Temp 75</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>5</v>
+      </c>
+      <c r="B46" t="str">
+        <v>ARMxl</v>
+      </c>
+      <c r="C46" t="str">
+        <v>stop_charge_session.sh</v>
+      </c>
+      <c r="D46" t="str">
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>5</v>
+      </c>
+      <c r="B47" t="str">
+        <v>AC_Source</v>
+      </c>
+      <c r="C47" t="str">
+        <v>set_output</v>
+      </c>
+      <c r="D47" t="str">
+        <v>OFF</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>5</v>
+      </c>
+      <c r="B48" t="str">
+        <v>DC_Source</v>
+      </c>
+      <c r="C48" t="str">
+        <v xml:space="preserve">set_output </v>
+      </c>
+      <c r="D48" t="str">
+        <v>OFF</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>5</v>
+      </c>
+      <c r="B49" t="str">
+        <v>CLIM_chamber</v>
+      </c>
+      <c r="C49" t="str">
+        <v>write_setpoint</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Temp 25</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D49"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1451,7 +1916,7 @@
         <v xml:space="preserve">set_output </v>
       </c>
       <c r="C15" t="str">
-        <v xml:space="preserve">set_output </v>
+        <v>set_output</v>
       </c>
       <c r="D15" t="str">
         <v>set_output</v>
@@ -1460,7 +1925,7 @@
         <v>set_voltage_and_power.sh</v>
       </c>
       <c r="F15" t="str">
-        <v xml:space="preserve">set_output </v>
+        <v>set_output</v>
       </c>
       <c r="G15" t="str">
         <v>save_screen</v>
@@ -1474,13 +1939,13 @@
         <v>set_function</v>
       </c>
       <c r="D16" t="str">
-        <v xml:space="preserve">set_frequency </v>
+        <v>set_frequency</v>
       </c>
       <c r="E16" t="str">
         <v>start_charge_session.sh</v>
       </c>
       <c r="F16" t="str">
-        <v xml:space="preserve">set_current </v>
+        <v>set_current</v>
       </c>
     </row>
     <row r="17">
@@ -1488,10 +1953,10 @@
         <v>stop_temp</v>
       </c>
       <c r="C17" t="str">
-        <v xml:space="preserve">set_voltage </v>
+        <v>set_voltage</v>
       </c>
       <c r="D17" t="str">
-        <v xml:space="preserve">set_voltage </v>
+        <v>set_voltage</v>
       </c>
       <c r="E17" t="str">
         <v>stop_charge_session.sh</v>
@@ -1505,7 +1970,7 @@
         <v>start_hum</v>
       </c>
       <c r="C18" t="str">
-        <v xml:space="preserve">set_c_limit </v>
+        <v>set_c_limit</v>
       </c>
       <c r="D18" t="str">
         <v>europe_grid</v>

</xml_diff>

<commit_message>
Update Readme Fix cycle_script bug for file selection Add repetitins for sequence
</commit_message>
<xml_diff>
--- a/command.xlsx
+++ b/command.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itdvtva\Desktop\7_Python-APP TEST\sequential_script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abb-my.sharepoint.com/personal/samuele_gonnelli_it_abb_com/Documents/Project/ARES_project/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_CE476470B5C54BA7A7B756B371AEF29B6F7CF196" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84429EC4-4C64-4D77-8966-C19C69406865}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SequenceConfig" sheetId="3" r:id="rId1"/>
@@ -275,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -933,12 +934,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -949,9 +944,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1262,22 +1263,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34">
         <v>5</v>
       </c>
@@ -1306,7 +1307,7 @@
       </c>
       <c r="E2" s="54"/>
     </row>
-    <row r="3" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="35">
         <v>5</v>
       </c>
@@ -1321,7 +1322,7 @@
       </c>
       <c r="E3" s="54"/>
     </row>
-    <row r="4" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35">
         <v>5</v>
       </c>
@@ -1336,7 +1337,7 @@
       </c>
       <c r="E4" s="54"/>
     </row>
-    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35">
         <v>5</v>
       </c>
@@ -1351,7 +1352,7 @@
       </c>
       <c r="E5" s="54"/>
     </row>
-    <row r="6" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="35">
         <v>5</v>
       </c>
@@ -1366,7 +1367,7 @@
       </c>
       <c r="E6" s="54"/>
     </row>
-    <row r="7" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="34">
         <v>5</v>
       </c>
@@ -1381,7 +1382,7 @@
       </c>
       <c r="E7" s="56"/>
     </row>
-    <row r="8" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36">
         <v>5</v>
       </c>
@@ -1396,7 +1397,7 @@
       </c>
       <c r="E8" s="56"/>
     </row>
-    <row r="9" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="34">
         <v>5</v>
       </c>
@@ -1411,7 +1412,7 @@
       </c>
       <c r="E9" s="56"/>
     </row>
-    <row r="10" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="35">
         <v>5</v>
       </c>
@@ -1426,7 +1427,7 @@
       </c>
       <c r="E10" s="56"/>
     </row>
-    <row r="11" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="50">
         <v>5</v>
       </c>
@@ -1441,7 +1442,7 @@
       </c>
       <c r="E11" s="44"/>
     </row>
-    <row r="12" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="51">
         <v>5</v>
       </c>
@@ -1456,7 +1457,7 @@
       </c>
       <c r="E12" s="44"/>
     </row>
-    <row r="13" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51">
         <v>5</v>
       </c>
@@ -1471,7 +1472,7 @@
       </c>
       <c r="E13" s="44"/>
     </row>
-    <row r="14" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51">
         <v>10</v>
       </c>
@@ -1486,7 +1487,7 @@
       </c>
       <c r="E14" s="44"/>
     </row>
-    <row r="15" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="51">
         <v>10</v>
       </c>
@@ -1501,7 +1502,7 @@
       </c>
       <c r="E15" s="44"/>
     </row>
-    <row r="16" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="51">
         <v>5</v>
       </c>
@@ -1516,24 +1517,24 @@
       </c>
       <c r="E16" s="44"/>
     </row>
-    <row r="17" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="52">
         <v>5</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="62" t="s">
+      <c r="C17" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="61" t="s">
         <v>5</v>
       </c>
       <c r="E17" s="44"/>
     </row>
-    <row r="18" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>55</v>
@@ -1546,9 +1547,9 @@
       </c>
       <c r="E18" s="44"/>
     </row>
-    <row r="19" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="58">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>55</v>
@@ -1561,22 +1562,22 @@
       </c>
       <c r="E19" s="44"/>
     </row>
-    <row r="20" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="50">
         <v>5</v>
       </c>
-      <c r="B20" s="64" t="s">
+      <c r="B20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="C20" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="64" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="55"/>
     </row>
-    <row r="21" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="52">
         <v>5</v>
       </c>
@@ -1591,7 +1592,7 @@
       </c>
       <c r="E21" s="55"/>
     </row>
-    <row r="22" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="51">
         <v>5</v>
       </c>
@@ -1606,7 +1607,7 @@
       </c>
       <c r="E22" s="55"/>
     </row>
-    <row r="23" spans="1:5" s="30" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" s="30" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="52">
         <v>10</v>
       </c>
@@ -1624,7 +1625,7 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C17 C20:C23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C17 C20:C23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>INDIRECT($B2)</formula1>
     </dataValidation>
   </dataValidations>
@@ -1633,7 +1634,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>CommandList!$B$14:$I$14</xm:f>
           </x14:formula1>
@@ -1646,7 +1647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1656,60 +1657,60 @@
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="59" t="s">
+    <row r="1" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="59" t="s">
+      <c r="C2" s="66"/>
+      <c r="D2" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="60"/>
-      <c r="F2" s="59" t="s">
+      <c r="E2" s="66"/>
+      <c r="F2" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="60"/>
-      <c r="H2" s="59" t="s">
+      <c r="G2" s="66"/>
+      <c r="H2" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="60"/>
-      <c r="J2" s="59" t="s">
+      <c r="I2" s="66"/>
+      <c r="J2" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="60"/>
-      <c r="L2" s="59" t="s">
+      <c r="K2" s="66"/>
+      <c r="L2" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="60"/>
-      <c r="N2" s="59" t="s">
+      <c r="M2" s="66"/>
+      <c r="N2" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="59" t="s">
+      <c r="O2" s="66"/>
+      <c r="P2" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="Q2" s="60"/>
-    </row>
-    <row r="3" spans="2:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q2" s="66"/>
+    </row>
+    <row r="3" spans="2:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
@@ -1759,7 +1760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>25</v>
       </c>
@@ -1809,7 +1810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="11"/>
       <c r="C5" s="5"/>
       <c r="D5" s="11" t="s">
@@ -1847,7 +1848,7 @@
       <c r="P5" s="11"/>
       <c r="Q5" s="7"/>
     </row>
-    <row r="6" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="5"/>
       <c r="D6" s="12" t="s">
@@ -1885,7 +1886,7 @@
       <c r="P6" s="12"/>
       <c r="Q6" s="7"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="12"/>
       <c r="C7" s="5"/>
       <c r="D7" s="12" t="s">
@@ -1919,7 +1920,7 @@
       <c r="P7" s="12"/>
       <c r="Q7" s="7"/>
     </row>
-    <row r="8" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="5"/>
       <c r="D8" s="12" t="s">
@@ -1953,7 +1954,7 @@
       <c r="P8" s="15"/>
       <c r="Q8" s="7"/>
     </row>
-    <row r="9" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="5"/>
       <c r="D9" s="12" t="s">
@@ -1983,7 +1984,7 @@
       <c r="P9" s="15"/>
       <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="2:17" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
       <c r="C10" s="5"/>
       <c r="D10" s="12" t="s">
@@ -2005,7 +2006,7 @@
       <c r="P10" s="20"/>
       <c r="Q10" s="21"/>
     </row>
-    <row r="11" spans="2:17" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
       <c r="C11" s="8"/>
       <c r="D11" s="13" t="s">
@@ -2027,7 +2028,7 @@
       <c r="P11" s="14"/>
       <c r="Q11" s="10"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="28" t="s">
         <v>7</v>
       </c>
@@ -2053,7 +2054,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B15" s="29" t="s">
         <v>5</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="2:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B16" s="1"/>
       <c r="C16" s="24" t="s">
         <v>16</v>
@@ -2099,7 +2100,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="24"/>
     </row>
-    <row r="17" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="24" t="s">
         <v>20</v>
@@ -2119,7 +2120,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="24"/>
     </row>
-    <row r="18" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="1"/>
       <c r="C18" s="24" t="s">
         <v>36</v>
@@ -2137,7 +2138,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="24"/>
     </row>
-    <row r="19" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B19" s="1"/>
       <c r="C19" s="24" t="s">
         <v>38</v>
@@ -2155,7 +2156,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="24"/>
     </row>
-    <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="24" t="s">
         <v>40</v>
@@ -2171,7 +2172,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="31"/>
     </row>
-    <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="24" t="s">
         <v>42</v>
@@ -2183,7 +2184,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="31"/>
     </row>
-    <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="24" t="s">
         <v>9</v>
@@ -2195,7 +2196,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="31"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="1"/>
       <c r="C23" s="24"/>
       <c r="D23" s="1"/>
@@ -2205,7 +2206,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="31"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="24"/>
       <c r="D24" s="1"/>

</xml_diff>